<commit_message>
README 파일 수정 및 start.py -> first_start.py로 수정
</commit_message>
<xml_diff>
--- a/1차_가공/경희대학교 국제캠퍼스 22년 1학기 1차 가공 완료.xlsx
+++ b/1차_가공/경희대학교 국제캠퍼스 22년 1학기 1차 가공 완료.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17974" uniqueCount="6416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17972" uniqueCount="6416">
   <si>
     <t>대학교명</t>
   </si>
@@ -19619,7 +19619,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L2089"/>
+  <dimension ref="A1:L2088"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -94586,17 +94586,6 @@
         <v>5998</v>
       </c>
     </row>
-    <row r="2089" spans="1:12">
-      <c r="A2089" s="1">
-        <v>2087</v>
-      </c>
-      <c r="B2089" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2089" t="s">
-        <v>12</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>